<commit_message>
Clean Directory, Finish final presentation
</commit_message>
<xml_diff>
--- a/Docs/featureRank_Check.xlsx
+++ b/Docs/featureRank_Check.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zzh94\Desktop\Repo\phishing_Detect\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9BCB723C-9D75-4A73-9B3E-F40C88C3129C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{D241E109-C472-4D02-801D-5A91F3138259}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12300" windowHeight="5715" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="41">
   <si>
     <t>Feature Position</t>
   </si>
@@ -156,6 +156,14 @@
   </si>
   <si>
     <t>Count</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>TPR</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>FPR</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -2763,31 +2771,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" altLang="zh-CN"/>
-              <a:t>RoC</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2839,7 +2822,9 @@
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -2866,19 +2851,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="1">
-                  <c:v>0.44642857142857145</c:v>
+                  <c:v>0.53030303030303028</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.18181818181818182</c:v>
+                  <c:v>0.24242424242424243</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.5326633165829151E-2</c:v>
+                  <c:v>6.0606060606060608E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.4925124792013313E-2</c:v>
+                  <c:v>3.3670033670033669E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.9669421487603308E-2</c:v>
+                  <c:v>2.1885521885521887E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2890,19 +2875,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="1">
-                  <c:v>0.42831215970961889</c:v>
+                  <c:v>0.51193058568329719</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.71485148514851482</c:v>
+                  <c:v>0.7830802603036876</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.92139737991266379</c:v>
+                  <c:v>0.91540130151843813</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.95594713656387664</c:v>
+                  <c:v>0.9414316702819957</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.97111111111111115</c:v>
+                  <c:v>0.94793926247288507</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2910,7 +2895,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-B5C2-4CB0-82EA-15AEC1E5C40A}"/>
+              <c16:uniqueId val="{00000000-07E9-41CF-BC0C-CD01617B8257}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2922,11 +2907,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="499022976"/>
-        <c:axId val="499025928"/>
+        <c:axId val="516743280"/>
+        <c:axId val="516745576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="499022976"/>
+        <c:axId val="516743280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2983,15 +2968,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="499025928"/>
+        <c:crossAx val="516745576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="499025928"/>
+        <c:axId val="516745576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3046,7 +3030,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="499022976"/>
+        <c:crossAx val="516743280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6616,23 +6600,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>14287</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>357187</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>471487</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>128587</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CE4FD4A-2593-45AF-9B9F-4BCAD9A2BD4C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{545D8FCF-9F75-40CE-9930-1474D4D7556E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6952,7 +6936,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U48"/>
   <sheetViews>
-    <sheetView topLeftCell="E28" workbookViewId="0">
+    <sheetView topLeftCell="E37" workbookViewId="0">
       <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
@@ -7016,7 +7000,7 @@
     </row>
     <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A3">
-        <f>SUM(A2+1)</f>
+        <f t="shared" ref="A3:A31" si="0">SUM(A2+1)</f>
         <v>2</v>
       </c>
       <c r="B3" s="1">
@@ -7053,7 +7037,7 @@
     </row>
     <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A4">
-        <f>SUM(A3+1)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B4" s="1">
@@ -7090,7 +7074,7 @@
     </row>
     <row r="5" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f>SUM(A4+1)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B5" s="2">
@@ -7127,7 +7111,7 @@
     </row>
     <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A6">
-        <f>SUM(A5+1)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B6" s="1">
@@ -7164,7 +7148,7 @@
     </row>
     <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A7">
-        <f>SUM(A6+1)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B7" s="1">
@@ -7201,7 +7185,7 @@
     </row>
     <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A8">
-        <f>SUM(A7+1)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B8" s="1">
@@ -7216,7 +7200,7 @@
     </row>
     <row r="9" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A9">
-        <f>SUM(A8+1)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B9" s="1">
@@ -7238,7 +7222,7 @@
     </row>
     <row r="10" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A10">
-        <f>SUM(A9+1)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B10" s="1">
@@ -7263,7 +7247,7 @@
     </row>
     <row r="11" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A11">
-        <f>SUM(A10+1)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B11" s="1">
@@ -7288,7 +7272,7 @@
     </row>
     <row r="12" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A12">
-        <f>SUM(A11+1)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B12" s="1">
@@ -7313,7 +7297,7 @@
     </row>
     <row r="13" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A13">
-        <f>SUM(A12+1)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B13" s="1">
@@ -7338,7 +7322,7 @@
     </row>
     <row r="14" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A14">
-        <f>SUM(A13+1)</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B14" s="1">
@@ -7363,7 +7347,7 @@
     </row>
     <row r="15" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A15">
-        <f>SUM(A14+1)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B15" s="1">
@@ -7378,7 +7362,7 @@
     </row>
     <row r="16" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A16">
-        <f>SUM(A15+1)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B16" s="1">
@@ -7393,7 +7377,7 @@
     </row>
     <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A17">
-        <f>SUM(A16+1)</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B17" s="1">
@@ -7408,7 +7392,7 @@
     </row>
     <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A18">
-        <f>SUM(A17+1)</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B18" s="1">
@@ -7420,7 +7404,7 @@
     </row>
     <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A19">
-        <f>SUM(A18+1)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="B19" s="1">
@@ -7432,7 +7416,7 @@
     </row>
     <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A20">
-        <f>SUM(A19+1)</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="B20" s="1">
@@ -7444,7 +7428,7 @@
     </row>
     <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A21">
-        <f>SUM(A20+1)</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="B21" s="1">
@@ -7456,7 +7440,7 @@
     </row>
     <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A22">
-        <f>SUM(A21+1)</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="B22" s="1">
@@ -7468,7 +7452,7 @@
     </row>
     <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A23">
-        <f>SUM(A22+1)</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="B23" s="1">
@@ -7480,7 +7464,7 @@
     </row>
     <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24">
-        <f>SUM(A23+1)</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="B24" s="1">
@@ -7492,7 +7476,7 @@
     </row>
     <row r="25" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A25">
-        <f>SUM(A24+1)</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="B25" s="1">
@@ -7504,7 +7488,7 @@
     </row>
     <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A26">
-        <f>SUM(A25+1)</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="B26" s="1">
@@ -7516,7 +7500,7 @@
     </row>
     <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A27">
-        <f>SUM(A26+1)</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="B27" s="1">
@@ -7528,7 +7512,7 @@
     </row>
     <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A28">
-        <f>SUM(A27+1)</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="B28" s="1">
@@ -7540,7 +7524,7 @@
     </row>
     <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A29">
-        <f>SUM(A28+1)</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="B29" s="1">
@@ -7552,7 +7536,7 @@
     </row>
     <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A30">
-        <f>SUM(A29+1)</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="B30" s="1">
@@ -7564,7 +7548,7 @@
     </row>
     <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A31">
-        <f>SUM(A30+1)</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="B31" s="1">
@@ -7890,8 +7874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D22E5C98-6ADC-4A03-9614-AA9A6B56E17E}">
   <dimension ref="C7:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G10" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -7923,10 +7907,10 @@
         <v>26</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="N7" s="5" t="s">
         <v>16</v>
@@ -7966,21 +7950,21 @@
         <v>236</v>
       </c>
       <c r="I9" s="5">
-        <v>315</v>
+        <v>225</v>
       </c>
       <c r="J9" s="5">
         <v>279</v>
       </c>
       <c r="K9" s="5">
-        <v>225</v>
+        <v>315</v>
       </c>
       <c r="L9" s="5">
-        <f>K9 /( SUM(J9:K9))</f>
-        <v>0.44642857142857145</v>
+        <f>K9/(SUM(J9,K9))</f>
+        <v>0.53030303030303028</v>
       </c>
       <c r="M9" s="5">
-        <f>H9/(SUM(H9:I9))</f>
-        <v>0.42831215970961889</v>
+        <f>H9/ SUM(H9,I9)</f>
+        <v>0.51193058568329719</v>
       </c>
       <c r="N9" s="5">
         <f xml:space="preserve"> (SUM(H9,J9))/1055</f>
@@ -8007,24 +7991,24 @@
         <v>361</v>
       </c>
       <c r="I10" s="5">
-        <v>144</v>
+        <v>100</v>
       </c>
       <c r="J10" s="5">
         <v>450</v>
       </c>
       <c r="K10" s="5">
-        <v>100</v>
+        <v>144</v>
       </c>
       <c r="L10" s="5">
-        <f t="shared" ref="L10:L13" si="0">K10 /( SUM(J10:K10))</f>
-        <v>0.18181818181818182</v>
+        <f>K10/(SUM(J10,K10))</f>
+        <v>0.24242424242424243</v>
       </c>
       <c r="M10" s="5">
-        <f>H10/(SUM(H10:I10))</f>
-        <v>0.71485148514851482</v>
+        <f>H10 /( SUM(H10,I10))</f>
+        <v>0.7830802603036876</v>
       </c>
       <c r="N10" s="5">
-        <f t="shared" ref="N10:N13" si="1" xml:space="preserve"> (SUM(H10,J10))/1055</f>
+        <f t="shared" ref="N10:N13" si="0" xml:space="preserve"> (SUM(H10,J10))/1055</f>
         <v>0.76872037914691949</v>
       </c>
     </row>
@@ -8048,24 +8032,24 @@
         <v>422</v>
       </c>
       <c r="I11" s="5">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="J11" s="5">
         <v>558</v>
       </c>
       <c r="K11" s="5">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="L11" s="5">
+        <f>K11/(SUM(J11,K11))</f>
+        <v>6.0606060606060608E-2</v>
+      </c>
+      <c r="M11" s="5">
+        <f>H11 /( SUM(H11,I11))</f>
+        <v>0.91540130151843813</v>
+      </c>
+      <c r="N11" s="5">
         <f t="shared" si="0"/>
-        <v>6.5326633165829151E-2</v>
-      </c>
-      <c r="M11" s="5">
-        <f t="shared" ref="M11:M13" si="2">H11/(SUM(H11:I11))</f>
-        <v>0.92139737991266379</v>
-      </c>
-      <c r="N11" s="5">
-        <f t="shared" si="1"/>
         <v>0.92890995260663511</v>
       </c>
     </row>
@@ -8089,24 +8073,24 @@
         <v>434</v>
       </c>
       <c r="I12" s="5">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="J12" s="5">
         <v>574</v>
       </c>
       <c r="K12" s="5">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="L12" s="5">
+        <f>K12/(SUM(J12,K12))</f>
+        <v>3.3670033670033669E-2</v>
+      </c>
+      <c r="M12" s="5">
+        <f>H12 /( SUM(H12,I12))</f>
+        <v>0.9414316702819957</v>
+      </c>
+      <c r="N12" s="5">
         <f t="shared" si="0"/>
-        <v>4.4925124792013313E-2</v>
-      </c>
-      <c r="M12" s="5">
-        <f t="shared" si="2"/>
-        <v>0.95594713656387664</v>
-      </c>
-      <c r="N12" s="5">
-        <f t="shared" si="1"/>
         <v>0.95545023696682463</v>
       </c>
     </row>
@@ -8130,24 +8114,24 @@
         <v>437</v>
       </c>
       <c r="I13" s="5">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="J13" s="5">
         <v>581</v>
       </c>
       <c r="K13" s="5">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="L13" s="5">
+        <f>K13/(SUM(J13,K13))</f>
+        <v>2.1885521885521887E-2</v>
+      </c>
+      <c r="M13" s="5">
+        <f>H13 /( SUM(H13,I13))</f>
+        <v>0.94793926247288507</v>
+      </c>
+      <c r="N13" s="5">
         <f t="shared" si="0"/>
-        <v>3.9669421487603308E-2</v>
-      </c>
-      <c r="M13" s="5">
-        <f t="shared" si="2"/>
-        <v>0.97111111111111115</v>
-      </c>
-      <c r="N13" s="5">
-        <f t="shared" si="1"/>
         <v>0.96492890995260661</v>
       </c>
     </row>

</xml_diff>